<commit_message>
Adaptación al refactor 🤩🤩🤩
</commit_message>
<xml_diff>
--- a/docs/source/_static/Resultados.xlsx
+++ b/docs/source/_static/Resultados.xlsx
@@ -10,13 +10,15 @@
     <sheet name="Ronda 1" sheetId="1" r:id="rId1"/>
     <sheet name="Clasificación" sheetId="2" r:id="rId2"/>
     <sheet name="Menciones" sheetId="3" r:id="rId3"/>
+    <sheet name="Jueces" sheetId="4" r:id="rId4"/>
+    <sheet name="Estadísticas" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="226">
   <si>
     <t>Sala</t>
   </si>
@@ -33,10 +35,10 @@
     <t>Alcázar de los Reyes Cristianos</t>
   </si>
   <si>
-    <t>ISDE (18)</t>
-  </si>
-  <si>
-    <t>ADUEEE (17.5)</t>
+    <t>CDU (18)</t>
+  </si>
+  <si>
+    <t>UJA (17)</t>
   </si>
   <si>
     <r>
@@ -48,7 +50,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez ADUMA</t>
+      <t>Juez UAL</t>
     </r>
     <r>
       <rPr>
@@ -58,17 +60,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez Rhētorica</t>
+      <t>, Juez ADUEEE</t>
     </r>
   </si>
   <si>
     <t>Calleja de las Flores</t>
   </si>
   <si>
-    <t>UPF (19)</t>
-  </si>
-  <si>
-    <t>ESADE (20)</t>
+    <t>ADA (17)</t>
+  </si>
+  <si>
+    <t>ADUEEE (18)</t>
   </si>
   <si>
     <r>
@@ -80,7 +82,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez ADUZ</t>
+      <t>Juez UJA</t>
     </r>
     <r>
       <rPr>
@@ -90,17 +92,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez SAFA</t>
+      <t>, Juez Comillas</t>
     </r>
   </si>
   <si>
     <t>Iglesia de Santa Marina</t>
   </si>
   <si>
-    <t>ADUSAL</t>
-  </si>
-  <si>
-    <t>ADUZ</t>
+    <t>UFV</t>
+  </si>
+  <si>
+    <t>SAFA</t>
   </si>
   <si>
     <r>
@@ -112,7 +114,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez CDUGR</t>
+      <t>Juez UC3M</t>
     </r>
     <r>
       <rPr>
@@ -122,17 +124,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez URJC</t>
+      <t>, Juez CEU San Pablo</t>
     </r>
   </si>
   <si>
     <t>La Judería</t>
   </si>
   <si>
-    <t>Comillas</t>
-  </si>
-  <si>
-    <t>Loyola</t>
+    <t>ISDE</t>
+  </si>
+  <si>
+    <t>ADUSAL</t>
   </si>
   <si>
     <r>
@@ -144,7 +146,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez CDU</t>
+      <t>Juez UFV</t>
     </r>
     <r>
       <rPr>
@@ -154,17 +156,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez Retórica</t>
+      <t>, Juez ADB</t>
     </r>
   </si>
   <si>
     <t>Medina Azahara</t>
   </si>
   <si>
-    <t>ADA</t>
-  </si>
-  <si>
-    <t>URJC</t>
+    <t>Loyola</t>
+  </si>
+  <si>
+    <t>Comillas</t>
   </si>
   <si>
     <r>
@@ -176,7 +178,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez CEU San Pablo</t>
+      <t>Juez URJC</t>
     </r>
     <r>
       <rPr>
@@ -186,17 +188,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez ISDE</t>
+      <t>, Juez CDUGR</t>
     </r>
   </si>
   <si>
     <t>Mezquita-Catedral</t>
   </si>
   <si>
-    <t>CEU San Pablo</t>
-  </si>
-  <si>
-    <t>CDU</t>
+    <t>URJC</t>
+  </si>
+  <si>
+    <t>ADUMA</t>
   </si>
   <si>
     <r>
@@ -208,7 +210,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez ADUEEE</t>
+      <t>Juez ESADE</t>
     </r>
     <r>
       <rPr>
@@ -218,17 +220,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez ESADE</t>
+      <t>, Juez ADUZ</t>
     </r>
   </si>
   <si>
     <t>Palacio de Viana</t>
   </si>
   <si>
-    <t>IEB</t>
-  </si>
-  <si>
     <t>UC3M</t>
+  </si>
+  <si>
+    <t>ADB</t>
   </si>
   <si>
     <r>
@@ -240,7 +242,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez ADB</t>
+      <t>Juez SAFA</t>
     </r>
     <r>
       <rPr>
@@ -250,17 +252,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez UJA</t>
+      <t>, Juez Dilema</t>
     </r>
   </si>
   <si>
     <t>Plaza de Capuchinos</t>
   </si>
   <si>
-    <t>UFV</t>
-  </si>
-  <si>
-    <t>Dilema</t>
+    <t>UPF</t>
+  </si>
+  <si>
+    <t>IEB</t>
   </si>
   <si>
     <r>
@@ -272,7 +274,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez Comillas</t>
+      <t>Juez ISDE</t>
     </r>
     <r>
       <rPr>
@@ -282,17 +284,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez UAL</t>
+      <t>, Juez ADA</t>
     </r>
   </si>
   <si>
     <t>Plaza de la Corredera</t>
   </si>
   <si>
-    <t>UAL</t>
-  </si>
-  <si>
-    <t>ADB</t>
+    <t>ESADE</t>
+  </si>
+  <si>
+    <t>Dilema</t>
   </si>
   <si>
     <r>
@@ -304,7 +306,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez Dilema</t>
+      <t>Juez Loyola</t>
     </r>
     <r>
       <rPr>
@@ -314,17 +316,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez UFV</t>
+      <t>, Juez Cánovas-UMA</t>
     </r>
   </si>
   <si>
     <t>Puente Romano</t>
   </si>
   <si>
-    <t>Cánovas-UMA</t>
-  </si>
-  <si>
-    <t>ADUMA</t>
+    <t>Uvigo</t>
+  </si>
+  <si>
+    <t>CEU San Pablo</t>
   </si>
   <si>
     <r>
@@ -336,7 +338,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez ADUSAL</t>
+      <t>Juez IEB</t>
     </r>
     <r>
       <rPr>
@@ -346,17 +348,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez Loyola</t>
+      <t>, Juez CDU</t>
     </r>
   </si>
   <si>
     <t>Puerta de Almodóvar</t>
   </si>
   <si>
-    <t>UJA</t>
-  </si>
-  <si>
-    <t>Uvigo</t>
+    <t>ADUZ</t>
+  </si>
+  <si>
+    <t>UAL</t>
   </si>
   <si>
     <r>
@@ -368,7 +370,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez Cánovas-UMA</t>
+      <t>Juez Retórica</t>
     </r>
     <r>
       <rPr>
@@ -378,7 +380,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez UC3M</t>
+      <t>, Juez ADUSAL</t>
     </r>
   </si>
   <si>
@@ -388,7 +390,7 @@
     <t>UGR</t>
   </si>
   <si>
-    <t>SAFA</t>
+    <t>Cánovas-UMA</t>
   </si>
   <si>
     <r>
@@ -400,7 +402,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Juez ADA</t>
+      <t>Juez Rhētorica</t>
     </r>
     <r>
       <rPr>
@@ -410,7 +412,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, Juez IEB</t>
+      <t>, Juez ADUMA</t>
     </r>
   </si>
   <si>
@@ -426,18 +428,27 @@
     <t>Media de ítems</t>
   </si>
   <si>
-    <t>ESADE</t>
-  </si>
-  <si>
-    <t>ISDE</t>
-  </si>
-  <si>
-    <t>UPF</t>
-  </si>
-  <si>
     <t>ADUEEE</t>
   </si>
   <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>ADA</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>UJA</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Nombre</t>
   </si>
   <si>
@@ -471,6 +482,9 @@
     <t>Orador 5</t>
   </si>
   <si>
+    <t>Orador 10</t>
+  </si>
+  <si>
     <t>Orador 6</t>
   </si>
   <si>
@@ -483,9 +497,6 @@
     <t>Orador 9</t>
   </si>
   <si>
-    <t>Orador 10</t>
-  </si>
-  <si>
     <t>Orador 11</t>
   </si>
   <si>
@@ -546,6 +557,51 @@
     <t>Orador 30</t>
   </si>
   <si>
+    <t>Orador 36</t>
+  </si>
+  <si>
+    <t>Orador 37</t>
+  </si>
+  <si>
+    <t>Orador 38</t>
+  </si>
+  <si>
+    <t>Orador 39</t>
+  </si>
+  <si>
+    <t>Orador 40</t>
+  </si>
+  <si>
+    <t>Orador 41</t>
+  </si>
+  <si>
+    <t>Orador 42</t>
+  </si>
+  <si>
+    <t>Orador 43</t>
+  </si>
+  <si>
+    <t>Orador 44</t>
+  </si>
+  <si>
+    <t>Orador 45</t>
+  </si>
+  <si>
+    <t>Orador 46</t>
+  </si>
+  <si>
+    <t>Orador 47</t>
+  </si>
+  <si>
+    <t>Orador 48</t>
+  </si>
+  <si>
+    <t>Orador 49</t>
+  </si>
+  <si>
+    <t>Orador 50</t>
+  </si>
+  <si>
     <t>Orador 31</t>
   </si>
   <si>
@@ -561,51 +617,6 @@
     <t>Orador 35</t>
   </si>
   <si>
-    <t>Orador 36</t>
-  </si>
-  <si>
-    <t>Orador 37</t>
-  </si>
-  <si>
-    <t>Orador 38</t>
-  </si>
-  <si>
-    <t>Orador 39</t>
-  </si>
-  <si>
-    <t>Orador 40</t>
-  </si>
-  <si>
-    <t>Orador 41</t>
-  </si>
-  <si>
-    <t>Orador 42</t>
-  </si>
-  <si>
-    <t>Orador 43</t>
-  </si>
-  <si>
-    <t>Orador 44</t>
-  </si>
-  <si>
-    <t>Orador 45</t>
-  </si>
-  <si>
-    <t>Orador 46</t>
-  </si>
-  <si>
-    <t>Orador 47</t>
-  </si>
-  <si>
-    <t>Orador 48</t>
-  </si>
-  <si>
-    <t>Orador 49</t>
-  </si>
-  <si>
-    <t>Orador 50</t>
-  </si>
-  <si>
     <t>Orador 51</t>
   </si>
   <si>
@@ -741,6 +752,9 @@
     <t>Orador 95</t>
   </si>
   <si>
+    <t>Orador 100</t>
+  </si>
+  <si>
     <t>Orador 96</t>
   </si>
   <si>
@@ -753,9 +767,6 @@
     <t>Orador 99</t>
   </si>
   <si>
-    <t>Orador 100</t>
-  </si>
-  <si>
     <t>Orador 101</t>
   </si>
   <si>
@@ -814,6 +825,117 @@
   </si>
   <si>
     <t>Orador 120</t>
+  </si>
+  <si>
+    <t>Juez</t>
+  </si>
+  <si>
+    <t>Juez ADA</t>
+  </si>
+  <si>
+    <t>UPF - IEB</t>
+  </si>
+  <si>
+    <t>Juez ADB</t>
+  </si>
+  <si>
+    <t>ISDE - ADUSAL</t>
+  </si>
+  <si>
+    <t>Juez ADUEEE</t>
+  </si>
+  <si>
+    <t>CDU (18.0) - UJA (17.0)</t>
+  </si>
+  <si>
+    <t>Juez ADUMA</t>
+  </si>
+  <si>
+    <t>UGR - Cánovas-UMA</t>
+  </si>
+  <si>
+    <t>Juez ADUSAL</t>
+  </si>
+  <si>
+    <t>ADUZ - UAL</t>
+  </si>
+  <si>
+    <t>Juez ADUZ</t>
+  </si>
+  <si>
+    <t>URJC - ADUMA</t>
+  </si>
+  <si>
+    <t>Juez Cánovas-UMA</t>
+  </si>
+  <si>
+    <t>ESADE - Dilema</t>
+  </si>
+  <si>
+    <t>Juez CDU</t>
+  </si>
+  <si>
+    <t>Uvigo - CEU San Pablo</t>
+  </si>
+  <si>
+    <t>Juez CDUGR</t>
+  </si>
+  <si>
+    <t>Loyola - Comillas</t>
+  </si>
+  <si>
+    <t>Juez CEU San Pablo</t>
+  </si>
+  <si>
+    <t>UFV - SAFA</t>
+  </si>
+  <si>
+    <t>Juez Comillas</t>
+  </si>
+  <si>
+    <t>ADA (17.0) - ADUEEE (18.0)</t>
+  </si>
+  <si>
+    <t>Juez Dilema</t>
+  </si>
+  <si>
+    <t>UC3M - ADB</t>
+  </si>
+  <si>
+    <t>Juez ESADE</t>
+  </si>
+  <si>
+    <t>Juez IEB</t>
+  </si>
+  <si>
+    <t>Juez ISDE</t>
+  </si>
+  <si>
+    <t>Juez Loyola</t>
+  </si>
+  <si>
+    <t>Juez Retórica</t>
+  </si>
+  <si>
+    <t>Juez Rhētorica</t>
+  </si>
+  <si>
+    <t>Juez SAFA</t>
+  </si>
+  <si>
+    <t>Juez UAL</t>
+  </si>
+  <si>
+    <t>Juez UC3M</t>
+  </si>
+  <si>
+    <t>Juez UFV</t>
+  </si>
+  <si>
+    <t>Juez UJA</t>
+  </si>
+  <si>
+    <t>Juez URJC</t>
   </si>
 </sst>
 </file>
@@ -857,12 +979,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,6 +995,49 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>365772</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>7629</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="pie_chart.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4267200" y="571500"/>
+          <a:ext cx="5852172" cy="4389129"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1164,9 +1332,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1386,410 +1554,410 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>20</v>
+      <c r="E2" s="3">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C3">
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3">
         <v>18</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5">
-        <v>17.5</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
       <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
+        <v>37</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
+      <c r="C15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
+      <c r="C20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
+        <v>13</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
+      <c r="C22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
+        <v>33</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
+        <v>25</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
+        <v>41</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1817,36 +1985,36 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1863,10 +2031,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1886,10 +2054,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1898,7 +2066,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -1909,10 +2077,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1927,15 +2095,15 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1955,10 +2123,10 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1978,10 +2146,10 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -2001,10 +2169,10 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2024,10 +2192,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2047,10 +2215,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2070,16 +2238,16 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2093,10 +2261,10 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -2108,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -2116,10 +2284,10 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -2139,10 +2307,10 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2154,7 +2322,7 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -2162,13 +2330,13 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -2185,10 +2353,10 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -2208,10 +2376,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2231,10 +2399,10 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -2254,10 +2422,10 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -2277,10 +2445,10 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2300,10 +2468,10 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2323,10 +2491,10 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -2346,10 +2514,10 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -2369,10 +2537,10 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2392,10 +2560,10 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -2415,10 +2583,10 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -2438,10 +2606,10 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2461,10 +2629,10 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -2484,10 +2652,10 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2507,10 +2675,10 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -2530,16 +2698,16 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -2553,10 +2721,10 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2568,7 +2736,7 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -2576,10 +2744,10 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2599,10 +2767,10 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2622,10 +2790,10 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2645,10 +2813,10 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2668,10 +2836,10 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2691,10 +2859,10 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2714,10 +2882,10 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2737,10 +2905,10 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2760,10 +2928,10 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2783,10 +2951,10 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2806,10 +2974,10 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2829,10 +2997,10 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2852,10 +3020,10 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2875,10 +3043,10 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2898,10 +3066,10 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2921,10 +3089,10 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2944,10 +3112,10 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2967,10 +3135,10 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2990,10 +3158,10 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -3013,10 +3181,10 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -3036,10 +3204,10 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B54" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -3059,10 +3227,10 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -3082,10 +3250,10 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B56" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -3105,10 +3273,10 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -3120,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -3128,10 +3296,10 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -3151,10 +3319,10 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -3163,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -3174,10 +3342,10 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -3197,13 +3365,13 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -3215,15 +3383,15 @@
         <v>0</v>
       </c>
       <c r="G61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B62" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -3243,10 +3411,10 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B63" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -3266,10 +3434,10 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B64" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -3289,10 +3457,10 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B65" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -3312,10 +3480,10 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B66" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -3335,10 +3503,10 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B67" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -3358,10 +3526,10 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B68" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -3381,10 +3549,10 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B69" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -3404,16 +3572,16 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B70" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -3427,10 +3595,10 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B71" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -3439,21 +3607,21 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71">
         <v>0</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B72" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -3473,10 +3641,10 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B73" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -3496,10 +3664,10 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B74" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -3519,10 +3687,10 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B75" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -3542,10 +3710,10 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -3565,10 +3733,10 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B77" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -3588,10 +3756,10 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B78" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -3611,10 +3779,10 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B79" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -3634,10 +3802,10 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B80" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -3657,10 +3825,10 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B81" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -3680,10 +3848,10 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B82" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -3703,10 +3871,10 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B83" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -3726,10 +3894,10 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B84" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -3749,10 +3917,10 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B85" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -3772,10 +3940,10 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B86" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -3795,10 +3963,10 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B87" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -3818,10 +3986,10 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B88" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -3841,10 +4009,10 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B89" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -3864,10 +4032,10 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B90" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -3887,10 +4055,10 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B91" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -3910,10 +4078,10 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B92" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -3933,10 +4101,10 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B93" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -3956,10 +4124,10 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B94" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -3979,10 +4147,10 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B95" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -4002,10 +4170,10 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B96" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -4025,7 +4193,7 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B97" t="s">
         <v>49</v>
@@ -4048,7 +4216,7 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B98" t="s">
         <v>49</v>
@@ -4071,7 +4239,7 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B99" t="s">
         <v>49</v>
@@ -4094,7 +4262,7 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B100" t="s">
         <v>49</v>
@@ -4117,7 +4285,7 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B101" t="s">
         <v>49</v>
@@ -4140,13 +4308,13 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B102" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -4163,10 +4331,10 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B103" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -4175,7 +4343,7 @@
         <v>0</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -4186,10 +4354,10 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B104" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -4204,15 +4372,15 @@
         <v>0</v>
       </c>
       <c r="G104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B105" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -4232,10 +4400,10 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B106" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -4255,10 +4423,10 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B107" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -4278,16 +4446,16 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B108" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C108">
         <v>0</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E108">
         <v>0</v>
@@ -4301,10 +4469,10 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B109" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -4324,10 +4492,10 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B110" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -4347,10 +4515,10 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B111" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -4370,10 +4538,10 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B112" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -4393,10 +4561,10 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B113" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -4416,10 +4584,10 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B114" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -4439,10 +4607,10 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B115" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -4462,10 +4630,10 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B116" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -4485,10 +4653,10 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B117" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -4508,10 +4676,10 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B118" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -4531,10 +4699,10 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B119" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -4554,10 +4722,10 @@
     </row>
     <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B120" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -4577,10 +4745,10 @@
     </row>
     <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B121" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -4601,4 +4769,234 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>